<commit_message>
New Add Category Problem History
</commit_message>
<xml_diff>
--- a/reports/ltb/1000455_Togle clamp patah/Togle clamp patah.xlsx
+++ b/reports/ltb/1000455_Togle clamp patah/Togle clamp patah.xlsx
@@ -7208,12 +7208,12 @@
       <c r="I35" s="116"/>
       <c r="J35" s="116"/>
       <c r="K35" s="117"/>
-      <c r="L35" s="258"/>
+      <c r="L35" s="258" t="s">
+        <v>83</v>
+      </c>
       <c r="M35" s="258"/>
       <c r="N35" s="258"/>
-      <c r="O35" s="258" t="s">
-        <v>83</v>
-      </c>
+      <c r="O35" s="258"/>
       <c r="P35" s="258"/>
       <c r="Q35" s="258"/>
       <c r="R35" s="258"/>

</xml_diff>